<commit_message>
first real work for RL2
</commit_message>
<xml_diff>
--- a/_other/WeekPlan.xlsx
+++ b/_other/WeekPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\exchange\RichLaughter2\_other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1305AED4-6B81-4995-85AA-EAAEEF748E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F0065D-3857-4EDD-9229-F670E76C19BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="348">
   <si>
     <t>Новый тест с использованием БД</t>
   </si>
@@ -1074,6 +1074,12 @@
   </si>
   <si>
     <t>QuikTrader (RL2)</t>
+  </si>
+  <si>
+    <t>Изменить время закрытия в QT (RL1)</t>
+  </si>
+  <si>
+    <t>grid_ranger (RL2)</t>
   </si>
 </sst>
 </file>
@@ -1531,9 +1537,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DF51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AI6" sqref="AI6"/>
+      <selection pane="bottomLeft" activeCell="AI4" sqref="AI4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2162,6 +2168,9 @@
       <c r="AG5" s="4" t="s">
         <v>344</v>
       </c>
+      <c r="AH5" s="2" t="s">
+        <v>346</v>
+      </c>
       <c r="AK5" s="2" t="s">
         <v>323</v>
       </c>
@@ -2583,6 +2592,9 @@
       </c>
       <c r="T12" s="7" t="s">
         <v>289</v>
+      </c>
+      <c r="AL12" s="2" t="s">
+        <v>347</v>
       </c>
       <c r="AM12" s="16" t="s">
         <v>294</v>

</xml_diff>

<commit_message>
some fix problem LWS2
</commit_message>
<xml_diff>
--- a/_other/WeekPlan.xlsx
+++ b/_other/WeekPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\exchange\RichLaughter2\_other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CCF223-6737-4D92-9CCB-7AC8C0E5B7BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D7F7F37-8CE4-4369-810D-637F2A0BCB8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="369">
   <si>
     <t>Новый тест с использованием БД</t>
   </si>
@@ -1147,6 +1147,9 @@
   </si>
   <si>
     <t>ST_mini парный (RL2)</t>
+  </si>
+  <si>
+    <t>Парный полу ST_mini полу LTA_KROSH. Один торгует лонг, другой шорт. Только взависимости от RSI &gt; 50 меняют стратегии</t>
   </si>
 </sst>
 </file>
@@ -1614,8 +1617,8 @@
   <dimension ref="A1:DF51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AK9" sqref="AK9"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AJ5" sqref="AJ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2200,8 +2203,11 @@
       <c r="AH4" s="19" t="s">
         <v>345</v>
       </c>
+      <c r="AI4" s="4" t="s">
+        <v>359</v>
+      </c>
       <c r="AL4" s="2" t="s">
-        <v>359</v>
+        <v>368</v>
       </c>
       <c r="AM4" s="2" t="s">
         <v>318</v>
@@ -2268,6 +2274,9 @@
       <c r="AH5" s="4" t="s">
         <v>346</v>
       </c>
+      <c r="AL5" s="2" t="s">
+        <v>352</v>
+      </c>
       <c r="AM5" s="2" t="s">
         <v>323</v>
       </c>
@@ -2290,7 +2299,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:110" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:110" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2338,6 +2347,9 @@
       </c>
       <c r="AH6" s="4" t="s">
         <v>348</v>
+      </c>
+      <c r="AL6" s="2" t="s">
+        <v>353</v>
       </c>
       <c r="AM6" s="2" t="s">
         <v>320</v>
@@ -2407,6 +2419,9 @@
       <c r="AH7" s="4" t="s">
         <v>349</v>
       </c>
+      <c r="AL7" s="2" t="s">
+        <v>354</v>
+      </c>
       <c r="AM7" s="2" t="s">
         <v>367</v>
       </c>
@@ -2773,9 +2788,6 @@
       <c r="T13" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="AM13" s="2" t="s">
-        <v>352</v>
-      </c>
       <c r="AO13" s="15" t="s">
         <v>258</v>
       </c>
@@ -2789,7 +2801,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="14" spans="1:110" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:110" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2825,9 +2837,6 @@
       </c>
       <c r="T14" s="4" t="s">
         <v>291</v>
-      </c>
-      <c r="AM14" s="2" t="s">
-        <v>353</v>
       </c>
       <c r="AO14" s="15" t="s">
         <v>268</v>
@@ -2875,9 +2884,6 @@
       </c>
       <c r="T15" s="7" t="s">
         <v>292</v>
-      </c>
-      <c r="AM15" s="2" t="s">
-        <v>354</v>
       </c>
       <c r="AO15" s="13" t="s">
         <v>281</v>

</xml_diff>